<commit_message>
Avance 13 - Marzo - 2017
</commit_message>
<xml_diff>
--- a/referencias/Rúbrica_Word_HCD.xlsx
+++ b/referencias/Rúbrica_Word_HCD.xlsx
@@ -413,18 +413,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -437,7 +426,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="6" builtinId="29"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -764,16 +764,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -786,156 +786,156 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
       <c r="I17" t="s">
         <v>45</v>
       </c>
@@ -944,13 +944,13 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="6">
         <v>10</v>
       </c>
@@ -962,13 +962,13 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="6">
         <v>9</v>
       </c>
@@ -980,13 +980,13 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="6">
         <v>7</v>
       </c>
@@ -995,13 +995,13 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="6">
         <v>4</v>
       </c>
@@ -1010,13 +1010,13 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="6">
         <v>1</v>
       </c>
@@ -1025,69 +1025,69 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="6">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
       <c r="G26" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="6">
         <v>6</v>
       </c>
@@ -1105,13 +1105,13 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
       <c r="G29" s="6">
         <v>5</v>
       </c>
@@ -1126,13 +1126,13 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
       <c r="G30" s="6">
         <v>4</v>
       </c>
@@ -1150,13 +1150,13 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="6">
         <v>2</v>
       </c>
@@ -1174,13 +1174,13 @@
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
       <c r="G32" s="6">
         <v>1</v>
       </c>
@@ -1195,38 +1195,38 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
       <c r="G34" s="5">
         <v>10</v>
       </c>
       <c r="I34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
       <c r="G35" s="5">
         <v>5</v>
       </c>
@@ -1235,39 +1235,39 @@
       </c>
     </row>
     <row r="36" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="5">
         <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
       <c r="L37" s="10"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
       <c r="G38" s="6">
         <v>10</v>
       </c>
@@ -1279,13 +1279,13 @@
       <c r="L38" s="10"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
       <c r="G39" s="6">
         <v>5</v>
       </c>
@@ -1297,17 +1297,17 @@
       <c r="L39" s="10"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
       <c r="G40" s="6">
         <v>1</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I40" s="11" t="s">
         <v>47</v>
       </c>
       <c r="J40" s="10"/>
@@ -1315,180 +1315,147 @@
       <c r="L40" s="10"/>
     </row>
     <row r="41" spans="2:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
       <c r="G42" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
       <c r="G43" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
       <c r="G44" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
       <c r="G45" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
       <c r="G46" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
       <c r="G48" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
       <c r="G49" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
       <c r="G50" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
       <c r="G51" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
       <c r="G52" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B51:F51"/>
@@ -1505,6 +1472,39 @@
     <mergeCell ref="B39:F39"/>
     <mergeCell ref="B40:F40"/>
     <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
13 - Marzo - 2017 Verifier: validateFooter Helper: class FooterResume
</commit_message>
<xml_diff>
--- a/referencias/Rúbrica_Word_HCD.xlsx
+++ b/referencias/Rúbrica_Word_HCD.xlsx
@@ -300,7 +300,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +321,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,7 +401,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -436,6 +442,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -754,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1212,10 +1221,10 @@
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
-      <c r="G34" s="5">
+      <c r="G34" s="20">
         <v>10</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1227,10 +1236,10 @@
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
-      <c r="G35" s="5">
+      <c r="G35" s="20">
         <v>5</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1242,10 +1251,10 @@
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
-      <c r="G36" s="5">
+      <c r="G36" s="20">
         <v>1</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="9" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>